<commit_message>
notes for set impact to spike
</commit_message>
<xml_diff>
--- a/Resources/Set Bonus for Spike.xlsx
+++ b/Resources/Set Bonus for Spike.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8B4C85-955E-419D-92C0-AA2BBBDBB567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0A3FE9-4B73-4F49-8489-CB5E51BF3C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{CC06AFE9-44C6-489A-8EE4-1B9D91154CC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Distance</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>clamp to 0-50?</t>
+  </si>
+  <si>
+    <t>or figure out how to adjust with the real range and an adjustment range</t>
   </si>
 </sst>
 </file>
@@ -1826,11 +1829,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DEA13E-050C-488A-B036-514181621061}">
-  <dimension ref="A1:L98"/>
+  <dimension ref="A1:L99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
+      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6080,6 +6083,11 @@
         <v>7</v>
       </c>
     </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
testing again 7-11 day
</commit_message>
<xml_diff>
--- a/Resources/Set Bonus for Spike.xlsx
+++ b/Resources/Set Bonus for Spike.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0A3FE9-4B73-4F49-8489-CB5E51BF3C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA7983E-C820-4FAB-A0AB-9A6BAFC42943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{CC06AFE9-44C6-489A-8EE4-1B9D91154CC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Distance</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>or figure out how to adjust with the real range and an adjustment range</t>
+  </si>
+  <si>
+    <t>I don't know</t>
   </si>
 </sst>
 </file>
@@ -1829,11 +1832,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DEA13E-050C-488A-B036-514181621061}">
-  <dimension ref="A1:L99"/>
+  <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
+      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6088,6 +6091,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A100" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Set effect for Spike for AI update idea
</commit_message>
<xml_diff>
--- a/Resources/Set Bonus for Spike.xlsx
+++ b/Resources/Set Bonus for Spike.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA7983E-C820-4FAB-A0AB-9A6BAFC42943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41759271-4F93-43F6-86D2-700CAE6F042B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{CC06AFE9-44C6-489A-8EE4-1B9D91154CC7}"/>
   </bookViews>
@@ -1512,6 +1512,364 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="10933762" cy="5945987"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFCAE6D2-0DAD-4AB4-83F3-3E1AB4471D7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="18690771"/>
+          <a:ext cx="10933762" cy="5945987"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Suggestion from Claude:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>private void TrySpike() {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    float jumpDuration = ai.JumpFrames / ai.AnimationFrameRate;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    float spikeDuration = ai.ActionFrames / ai.AnimationFrameRate;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    float optimalTime = spikeTime - jumpDuration - spikeDuration / 2;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    // Create a timing window around the optimal time</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    float timingWindow = ai.BallInfo.SkillValues.SkillToValue(ai.Skills.SpikeSkill, ai.BallInfo.SkillValues.SpikeTimingWindow);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    if (ai.BallInfo.TimeSinceLastHit &gt;= optimalTime - timingWindow &amp;&amp; </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        ai.BallInfo.TimeSinceLastHit &lt;= optimalTime + timingWindow &amp;&amp; </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        spikeTime &gt;= 0) {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        ai.PerformJump();</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        isSpiking = true;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        // Calculate timing variance similar to human system</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        // This should be a small value, similar to how human normalizedTime - 1 works</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        float timingDeviation = (ai.BallInfo.TimeSinceLastHit - optimalTime) / timingWindow;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        // Apply the same penalty calculation as humans</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        float window = ai.BallInfo.SkillValues.SkillToValue(ai.Skills.SpikeSkill, ai.BallInfo.SkillValues.SpikeTimingWindow);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        float penalty = timingDeviation * window * spikeWindowPenalty;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        ai.SpikeSpeedPenalty = timingDeviation * window; // This should be much smaller now</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>        Debug.Log($"AI Timing: deviation={timingDeviation:F3}, window={window:F3}, penalty={penalty:F3}");</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    }</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>}</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>The key changes:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>timingDeviation</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> is normalized to [-1, 1] range (perfect timing = 0)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Penalty calculation</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> mirrors the human system more closely</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" b="1"/>
+            <a:t>Values should be much smaller</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> since timingDeviation is constrained</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>This should give you penalties in a reasonable range (similar to what humans experience) rather than the 0.99+ values you're seeing. </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1835,8 +2193,8 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A134" sqref="A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Another suggestion from Claude after poking holes
Might ultimately need to practice with human controls and do super early, super late, and see how close to get on time and try to somehow replicate that for the AI
</commit_message>
<xml_diff>
--- a/Resources/Set Bonus for Spike.xlsx
+++ b/Resources/Set Bonus for Spike.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41759271-4F93-43F6-86D2-700CAE6F042B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB524B2-E619-4BF8-A7E4-2724FA7F90DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{CC06AFE9-44C6-489A-8EE4-1B9D91154CC7}"/>
   </bookViews>
@@ -1519,7 +1519,7 @@
       <xdr:row>101</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="10933762" cy="5945987"/>
+    <xdr:ext cx="10425931" cy="3523465"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="TextBox 2">
@@ -1534,7 +1534,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="18690771"/>
-          <a:ext cx="10933762" cy="5945987"/>
+          <a:ext cx="10425931" cy="3523465"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1563,7 +1563,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Suggestion from Claude:</a:t>
+            <a:t>New solution from Claude:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1575,7 +1575,7 @@
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>private void TrySpike() {</a:t>
+            <a:t>float optimalTime = spikeTime - jumpDuration - spikeDuration / 2;</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1584,30 +1584,90 @@
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    float jumpDuration = ai.JumpFrames / ai.AnimationFrameRate;</a:t>
+            <a:t>if (ai.BallInfo.TimeSinceLastHit &gt;= optimalTime &amp;&amp; spikeTime &gt;= 0) {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>If baseTimingError is ~0.995, that means the AI is waiting way too long before jumping. The timing should be much tighter.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US"/>
+            <a:t>Instead of trying to normalize a huge timing error, we should fix the AI to jump closer to the optimal time. Maybe something like:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    float spikeDuration = ai.ActionFrames / ai.AnimationFrameRate;</a:t>
+            <a:t>// Add small random variance around optimal time (like ±0.1 seconds max)</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    float optimalTime = spikeTime - jumpDuration - spikeDuration / 2;</a:t>
+            <a:t>float timingVariance = Random.Range(-0.05f, 0.05f); // Much smaller range</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>float targetTime = optimalTime + timingVariance;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US">
+            <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>if (ai.BallInfo.TimeSinceLastHit &gt;= targetTime &amp;&amp; spikeTime &gt;= 0) {</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    ai.PerformJump();</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>    isSpiking = true;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
@@ -1616,254 +1676,47 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    // Create a timing window around the optimal time</a:t>
+            <a:t>    // Now the timing error should be small (like human system)</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    float timingWindow = ai.BallInfo.SkillValues.SkillToValue(ai.Skills.SpikeSkill, ai.BallInfo.SkillValues.SpikeTimingWindow);</a:t>
+            <a:t>    float actualTimingError = ai.BallInfo.TimeSinceLastHit - optimalTime; // Should be ~0.05 or less</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    </a:t>
+            <a:t>    float window = ai.BallInfo.SkillValues.SkillToValue(ai.Skills.SpikeSkill, ai.BallInfo.SkillValues.SpikeTimingWindow);</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>    if (ai.BallInfo.TimeSinceLastHit &gt;= optimalTime - timingWindow &amp;&amp; </a:t>
+            <a:t>    ai.SpikeSpeedPenalty = actualTimingError * window;</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        ai.BallInfo.TimeSinceLastHit &lt;= optimalTime + timingWindow &amp;&amp; </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        spikeTime &gt;= 0) {</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        ai.PerformJump();</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        isSpiking = true;</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        // Calculate timing variance similar to human system</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        // This should be a small value, similar to how human normalizedTime - 1 works</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        float timingDeviation = (ai.BallInfo.TimeSinceLastHit - optimalTime) / timingWindow;</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        // Apply the same penalty calculation as humans</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        float window = ai.BallInfo.SkillValues.SkillToValue(ai.Skills.SpikeSkill, ai.BallInfo.SkillValues.SpikeTimingWindow);</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        float penalty = timingDeviation * window * spikeWindowPenalty;</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        ai.SpikeSpeedPenalty = timingDeviation * window; // This should be much smaller now</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>        Debug.Log($"AI Timing: deviation={timingDeviation:F3}, window={window:F3}, penalty={penalty:F3}");</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>    }</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
+            <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
             <a:t>}</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>The key changes:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" b="1"/>
-            <a:t>timingDeviation</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> is normalized to [-1, 1] range (perfect timing = 0)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" b="1"/>
-            <a:t>Penalty calculation</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> mirrors the human system more closely</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" b="1"/>
-            <a:t>Values should be much smaller</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t> since timingDeviation is constrained</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>This should give you penalties in a reasonable range (similar to what humans experience) rather than the 0.99+ values you're seeing. </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2193,8 +2046,8 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A134" sqref="A134"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Next to do for new set code
</commit_message>
<xml_diff>
--- a/Resources/Set Bonus for Spike.xlsx
+++ b/Resources/Set Bonus for Spike.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB524B2-E619-4BF8-A7E4-2724FA7F90DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3821AB90-A052-4779-8265-90F8A9FCA812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{CC06AFE9-44C6-489A-8EE4-1B9D91154CC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Distance</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>I don't know</t>
+  </si>
+  <si>
+    <t>Next up:  implement &amp; test!</t>
   </si>
 </sst>
 </file>
@@ -2043,11 +2046,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DEA13E-050C-488A-B036-514181621061}">
-  <dimension ref="A1:L100"/>
+  <dimension ref="A1:L122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A122" sqref="A122"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6307,6 +6310,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A122" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
More messages in testing file
</commit_message>
<xml_diff>
--- a/Resources/Set Bonus for Spike.xlsx
+++ b/Resources/Set Bonus for Spike.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3821AB90-A052-4779-8265-90F8A9FCA812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70A9187-0119-48FC-AF59-74AE0E3BFAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{CC06AFE9-44C6-489A-8EE4-1B9D91154CC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Distance</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Next up:  implement &amp; test!</t>
+  </si>
+  <si>
+    <t>Still no testing done.  Not into it.</t>
   </si>
 </sst>
 </file>
@@ -2046,11 +2049,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DEA13E-050C-488A-B036-514181621061}">
-  <dimension ref="A1:L122"/>
+  <dimension ref="A1:L123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A123" sqref="A123"/>
+      <selection pane="bottomLeft" activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6315,6 +6318,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A123" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Message in testing file (b)
</commit_message>
<xml_diff>
--- a/Resources/Set Bonus for Spike.xlsx
+++ b/Resources/Set Bonus for Spike.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70A9187-0119-48FC-AF59-74AE0E3BFAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00757E8-E77D-4EE4-AAD3-B2FCBD1D25AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{CC06AFE9-44C6-489A-8EE4-1B9D91154CC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Distance</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Still no testing done.  Not into it.</t>
+  </si>
+  <si>
+    <t>I can't do this anymore</t>
   </si>
 </sst>
 </file>
@@ -2049,11 +2052,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DEA13E-050C-488A-B036-514181621061}">
-  <dimension ref="A1:L123"/>
+  <dimension ref="A1:L124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A124" sqref="A124"/>
+      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6323,6 +6326,11 @@
         <v>11</v>
       </c>
     </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A124" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Message in testing file (c)
</commit_message>
<xml_diff>
--- a/Resources/Set Bonus for Spike.xlsx
+++ b/Resources/Set Bonus for Spike.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00757E8-E77D-4EE4-AAD3-B2FCBD1D25AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F24D41A-F53B-4A22-8EC2-6FE22A616D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{CC06AFE9-44C6-489A-8EE4-1B9D91154CC7}"/>
+    <workbookView xWindow="10346" yWindow="6943" windowWidth="22277" windowHeight="10594" xr2:uid="{CC06AFE9-44C6-489A-8EE4-1B9D91154CC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Distance</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>I can't do this anymore</t>
+  </si>
+  <si>
+    <t>almost there</t>
   </si>
 </sst>
 </file>
@@ -2052,11 +2055,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DEA13E-050C-488A-B036-514181621061}">
-  <dimension ref="A1:L124"/>
+  <dimension ref="A1:L125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -6331,6 +6334,11 @@
         <v>12</v>
       </c>
     </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A125" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Speed Penalty for AI (FI6ENWvK)
</commit_message>
<xml_diff>
--- a/Resources/Set Bonus for Spike.xlsx
+++ b/Resources/Set Bonus for Spike.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F24D41A-F53B-4A22-8EC2-6FE22A616D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA97FAE-48D6-4238-8605-28844525212A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10346" yWindow="6943" windowWidth="22277" windowHeight="10594" xr2:uid="{CC06AFE9-44C6-489A-8EE4-1B9D91154CC7}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{CC06AFE9-44C6-489A-8EE4-1B9D91154CC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Distance</t>
   </si>
@@ -79,6 +80,30 @@
   <si>
     <t>almost there</t>
   </si>
+  <si>
+    <t>time since last hit</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>optimal time</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>spike speed penalty</t>
+  </si>
+  <si>
+    <t>actual timing error</t>
+  </si>
 </sst>
 </file>
 
@@ -116,9 +141,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2057,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DEA13E-050C-488A-B036-514181621061}">
   <dimension ref="A1:L125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
@@ -6343,4 +6369,82 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D8B855-822A-4593-875E-B7215605D3B7}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.07421875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.4609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.84375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>0.92250149999999997</v>
+      </c>
+      <c r="C2">
+        <v>0.97702040000000001</v>
+      </c>
+      <c r="E2">
+        <f>A2-C2</f>
+        <v>-5.4518900000000037E-2</v>
+      </c>
+      <c r="G2">
+        <v>5.5555559999999997E-2</v>
+      </c>
+      <c r="I2">
+        <f>ABS(E2)*G2</f>
+        <v>3.0288280200840021E-3</v>
+      </c>
+      <c r="J2">
+        <f>A2-C2</f>
+        <v>-5.4518900000000037E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>